<commit_message>
Starting import from second line
</commit_message>
<xml_diff>
--- a/Content/GAZPROM ELEC FLAT.xlsx
+++ b/Content/GAZPROM ELEC FLAT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smb/Desktop/UTDS/Pricebooks_24_11_2020/Gazprom/Original Pricebooks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Renis Kraja\Desktop\Salesforce\Pricebooks_24_11_2020\Pricebooks_24_11_2020\Gazprom\Original Pricebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{925A5FC3-647E-DF4B-B1D0-88FE22A7FEEF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE82FC5A-41CB-475E-A7DA-A3E75513EB56}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="460" windowWidth="22860" windowHeight="14660" xr2:uid="{84039258-7006-4002-AB5C-BF2BA5AB5C4A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11280" xr2:uid="{84039258-7006-4002-AB5C-BF2BA5AB5C4A}"/>
   </bookViews>
   <sheets>
     <sheet name="Electricity" sheetId="1" r:id="rId1"/>
@@ -167,7 +167,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -596,27 +596,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47355293-2571-48F3-B9A3-CAC602E5367E}">
   <dimension ref="A1:L506"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A496" workbookViewId="0">
+      <selection activeCell="E502" sqref="E502"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="2.33203125" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" customWidth="1"/>
-    <col min="3" max="3" width="38.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="57.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.83203125" customWidth="1"/>
-    <col min="7" max="7" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="2.33203125" customWidth="1"/>
-    <col min="13" max="16384" width="9.1640625" hidden="1"/>
+    <col min="1" max="1" width="2.28515625" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="57.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="2.28515625" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="99" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:11" ht="99" customHeight="1">
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
@@ -648,7 +648,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="2:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:11" ht="45">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -680,7 +680,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:11">
       <c r="B3" s="2">
         <v>1</v>
       </c>
@@ -712,7 +712,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:11">
       <c r="B4" s="2">
         <v>1</v>
       </c>
@@ -744,7 +744,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:11">
       <c r="B5" s="2">
         <v>1</v>
       </c>
@@ -776,7 +776,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:11">
       <c r="B6" s="2">
         <v>1</v>
       </c>
@@ -808,7 +808,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:11">
       <c r="B7" s="2">
         <v>1</v>
       </c>
@@ -840,7 +840,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:11">
       <c r="B8" s="2">
         <v>1</v>
       </c>
@@ -872,7 +872,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:11">
       <c r="B9" s="2">
         <v>1</v>
       </c>
@@ -904,7 +904,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:11">
       <c r="B10" s="2">
         <v>1</v>
       </c>
@@ -936,7 +936,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:11">
       <c r="B11" s="2">
         <v>1</v>
       </c>
@@ -968,7 +968,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:11">
       <c r="B12" s="2">
         <v>1</v>
       </c>
@@ -1000,7 +1000,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:11">
       <c r="B13" s="2">
         <v>1</v>
       </c>
@@ -1032,7 +1032,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:11">
       <c r="B14" s="2">
         <v>1</v>
       </c>
@@ -1064,7 +1064,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:11">
       <c r="B15" s="2">
         <v>1</v>
       </c>
@@ -1096,7 +1096,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:11">
       <c r="B16" s="2">
         <v>1</v>
       </c>
@@ -1128,7 +1128,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:11">
       <c r="B17" s="2">
         <v>2</v>
       </c>
@@ -1160,7 +1160,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:11">
       <c r="B18" s="2">
         <v>2</v>
       </c>
@@ -1192,7 +1192,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:11">
       <c r="B19" s="2">
         <v>2</v>
       </c>
@@ -1224,7 +1224,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:11">
       <c r="B20" s="2">
         <v>2</v>
       </c>
@@ -1256,7 +1256,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:11">
       <c r="B21" s="2">
         <v>2</v>
       </c>
@@ -1288,7 +1288,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:11">
       <c r="B22" s="2">
         <v>2</v>
       </c>
@@ -1320,7 +1320,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:11">
       <c r="B23" s="2">
         <v>2</v>
       </c>
@@ -1352,7 +1352,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:11">
       <c r="B24" s="2">
         <v>2</v>
       </c>
@@ -1384,7 +1384,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:11">
       <c r="B25" s="2">
         <v>2</v>
       </c>
@@ -1416,7 +1416,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:11">
       <c r="B26" s="2">
         <v>2</v>
       </c>
@@ -1448,7 +1448,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:11">
       <c r="B27" s="2">
         <v>2</v>
       </c>
@@ -1480,7 +1480,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:11">
       <c r="B28" s="2">
         <v>2</v>
       </c>
@@ -1512,7 +1512,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:11">
       <c r="B29" s="2">
         <v>2</v>
       </c>
@@ -1544,7 +1544,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:11">
       <c r="B30" s="2">
         <v>2</v>
       </c>
@@ -1576,7 +1576,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:11">
       <c r="B31" s="2">
         <v>3</v>
       </c>
@@ -1608,7 +1608,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:11">
       <c r="B32" s="2">
         <v>3</v>
       </c>
@@ -1640,7 +1640,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:11">
       <c r="B33" s="2">
         <v>3</v>
       </c>
@@ -1672,7 +1672,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:11">
       <c r="B34" s="2">
         <v>3</v>
       </c>
@@ -1704,7 +1704,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:11">
       <c r="B35" s="2">
         <v>3</v>
       </c>
@@ -1736,7 +1736,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:11">
       <c r="B36" s="2">
         <v>3</v>
       </c>
@@ -1768,7 +1768,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:11">
       <c r="B37" s="2">
         <v>3</v>
       </c>
@@ -1800,7 +1800,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:11">
       <c r="B38" s="2">
         <v>3</v>
       </c>
@@ -1832,7 +1832,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:11">
       <c r="B39" s="2">
         <v>3</v>
       </c>
@@ -1864,7 +1864,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:11">
       <c r="B40" s="2">
         <v>3</v>
       </c>
@@ -1896,7 +1896,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:11">
       <c r="B41" s="2">
         <v>3</v>
       </c>
@@ -1928,7 +1928,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:11">
       <c r="B42" s="2">
         <v>3</v>
       </c>
@@ -1960,7 +1960,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:11">
       <c r="B43" s="2">
         <v>3</v>
       </c>
@@ -1992,7 +1992,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:11">
       <c r="B44" s="2">
         <v>3</v>
       </c>
@@ -2024,7 +2024,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:11">
       <c r="B45" s="2">
         <v>3</v>
       </c>
@@ -2056,7 +2056,7 @@
         <v>12.863702627845706</v>
       </c>
     </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:11">
       <c r="B46" s="2">
         <v>3</v>
       </c>
@@ -2088,7 +2088,7 @@
         <v>13.149999999999999</v>
       </c>
     </row>
-    <row r="47" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:11">
       <c r="B47" s="2">
         <v>3</v>
       </c>
@@ -2120,7 +2120,7 @@
         <v>12.22448822875619</v>
       </c>
     </row>
-    <row r="48" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:11">
       <c r="B48" s="2">
         <v>3</v>
       </c>
@@ -2152,7 +2152,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="49" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:11">
       <c r="B49" s="2">
         <v>3</v>
       </c>
@@ -2184,7 +2184,7 @@
         <v>13.6</v>
       </c>
     </row>
-    <row r="50" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:11">
       <c r="B50" s="2">
         <v>3</v>
       </c>
@@ -2216,7 +2216,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="51" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:11">
       <c r="B51" s="2">
         <v>3</v>
       </c>
@@ -2248,7 +2248,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:11">
       <c r="B52" s="2">
         <v>3</v>
       </c>
@@ -2280,7 +2280,7 @@
         <v>14.130000000000003</v>
       </c>
     </row>
-    <row r="53" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:11">
       <c r="B53" s="2">
         <v>3</v>
       </c>
@@ -2312,7 +2312,7 @@
         <v>13.169999999999998</v>
       </c>
     </row>
-    <row r="54" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:11">
       <c r="B54" s="2">
         <v>3</v>
       </c>
@@ -2344,7 +2344,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="55" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:11">
       <c r="B55" s="2">
         <v>3</v>
       </c>
@@ -2376,7 +2376,7 @@
         <v>13.338203359858536</v>
       </c>
     </row>
-    <row r="56" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:11">
       <c r="B56" s="2">
         <v>3</v>
       </c>
@@ -2408,7 +2408,7 @@
         <v>13.760198876575073</v>
       </c>
     </row>
-    <row r="57" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:11">
       <c r="B57" s="2">
         <v>3</v>
       </c>
@@ -2440,7 +2440,7 @@
         <v>13.97</v>
       </c>
     </row>
-    <row r="58" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:11">
       <c r="B58" s="2">
         <v>3</v>
       </c>
@@ -2472,7 +2472,7 @@
         <v>13.21</v>
       </c>
     </row>
-    <row r="59" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:11">
       <c r="B59" s="2">
         <v>4</v>
       </c>
@@ -2504,7 +2504,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="60" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:11">
       <c r="B60" s="2">
         <v>4</v>
       </c>
@@ -2536,7 +2536,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="61" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:11">
       <c r="B61" s="2">
         <v>4</v>
       </c>
@@ -2568,7 +2568,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="62" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:11">
       <c r="B62" s="2">
         <v>4</v>
       </c>
@@ -2600,7 +2600,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="63" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:11">
       <c r="B63" s="2">
         <v>4</v>
       </c>
@@ -2632,7 +2632,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="64" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:11">
       <c r="B64" s="2">
         <v>4</v>
       </c>
@@ -2664,7 +2664,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="65" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:11">
       <c r="B65" s="2">
         <v>4</v>
       </c>
@@ -2696,7 +2696,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="66" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:11">
       <c r="B66" s="2">
         <v>4</v>
       </c>
@@ -2728,7 +2728,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="67" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:11">
       <c r="B67" s="2">
         <v>4</v>
       </c>
@@ -2760,7 +2760,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="68" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:11">
       <c r="B68" s="2">
         <v>4</v>
       </c>
@@ -2792,7 +2792,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="69" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:11">
       <c r="B69" s="2">
         <v>4</v>
       </c>
@@ -2824,7 +2824,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="70" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:11">
       <c r="B70" s="2">
         <v>4</v>
       </c>
@@ -2856,7 +2856,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="71" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:11">
       <c r="B71" s="2">
         <v>4</v>
       </c>
@@ -2888,7 +2888,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="72" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:11">
       <c r="B72" s="2">
         <v>4</v>
       </c>
@@ -2920,7 +2920,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="73" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:11">
       <c r="B73" s="2">
         <v>4</v>
       </c>
@@ -2952,7 +2952,7 @@
         <v>13.140000000000002</v>
       </c>
     </row>
-    <row r="74" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:11">
       <c r="B74" s="2">
         <v>4</v>
       </c>
@@ -2984,7 +2984,7 @@
         <v>13.36</v>
       </c>
     </row>
-    <row r="75" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:11">
       <c r="B75" s="2">
         <v>4</v>
       </c>
@@ -3016,7 +3016,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="76" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:11">
       <c r="B76" s="2">
         <v>4</v>
       </c>
@@ -3048,7 +3048,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="77" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:11">
       <c r="B77" s="2">
         <v>4</v>
       </c>
@@ -3080,7 +3080,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="78" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:11">
       <c r="B78" s="2">
         <v>4</v>
       </c>
@@ -3112,7 +3112,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="79" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:11">
       <c r="B79" s="2">
         <v>4</v>
       </c>
@@ -3144,7 +3144,7 @@
         <v>13.58</v>
       </c>
     </row>
-    <row r="80" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:11">
       <c r="B80" s="2">
         <v>4</v>
       </c>
@@ -3176,7 +3176,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="81" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:11">
       <c r="B81" s="2">
         <v>4</v>
       </c>
@@ -3208,7 +3208,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="82" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:11">
       <c r="B82" s="2">
         <v>4</v>
       </c>
@@ -3240,7 +3240,7 @@
         <v>13.467242195909581</v>
       </c>
     </row>
-    <row r="83" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:11">
       <c r="B83" s="2">
         <v>4</v>
       </c>
@@ -3272,7 +3272,7 @@
         <v>13.896194690265485</v>
       </c>
     </row>
-    <row r="84" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:11">
       <c r="B84" s="2">
         <v>4</v>
       </c>
@@ -3304,7 +3304,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="85" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:11">
       <c r="B85" s="2">
         <v>4</v>
       </c>
@@ -3336,7 +3336,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="86" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:11">
       <c r="B86" s="2">
         <v>4</v>
       </c>
@@ -3368,7 +3368,7 @@
         <v>13.67</v>
       </c>
     </row>
-    <row r="87" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:11">
       <c r="B87" s="2">
         <v>1</v>
       </c>
@@ -3400,7 +3400,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="88" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:11">
       <c r="B88" s="2">
         <v>1</v>
       </c>
@@ -3432,7 +3432,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="89" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:11">
       <c r="B89" s="2">
         <v>1</v>
       </c>
@@ -3464,7 +3464,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="90" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:11">
       <c r="B90" s="2">
         <v>1</v>
       </c>
@@ -3496,7 +3496,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="91" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:11">
       <c r="B91" s="2">
         <v>1</v>
       </c>
@@ -3528,7 +3528,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="92" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="92" spans="2:11">
       <c r="B92" s="2">
         <v>1</v>
       </c>
@@ -3560,7 +3560,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="93" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="93" spans="2:11">
       <c r="B93" s="2">
         <v>1</v>
       </c>
@@ -3592,7 +3592,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="94" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="94" spans="2:11">
       <c r="B94" s="2">
         <v>1</v>
       </c>
@@ -3624,7 +3624,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="95" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="95" spans="2:11">
       <c r="B95" s="2">
         <v>1</v>
       </c>
@@ -3656,7 +3656,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="96" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="96" spans="2:11">
       <c r="B96" s="2">
         <v>1</v>
       </c>
@@ -3688,7 +3688,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="97" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:11">
       <c r="B97" s="2">
         <v>1</v>
       </c>
@@ -3720,7 +3720,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="98" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:11">
       <c r="B98" s="2">
         <v>1</v>
       </c>
@@ -3752,7 +3752,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="99" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:11">
       <c r="B99" s="2">
         <v>1</v>
       </c>
@@ -3784,7 +3784,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="100" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:11">
       <c r="B100" s="2">
         <v>1</v>
       </c>
@@ -3816,7 +3816,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="101" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:11">
       <c r="B101" s="2">
         <v>2</v>
       </c>
@@ -3848,7 +3848,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="102" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:11">
       <c r="B102" s="2">
         <v>2</v>
       </c>
@@ -3880,7 +3880,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="103" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:11">
       <c r="B103" s="2">
         <v>2</v>
       </c>
@@ -3912,7 +3912,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="104" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="104" spans="2:11">
       <c r="B104" s="2">
         <v>2</v>
       </c>
@@ -3944,7 +3944,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="105" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="105" spans="2:11">
       <c r="B105" s="2">
         <v>2</v>
       </c>
@@ -3976,7 +3976,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="106" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="106" spans="2:11">
       <c r="B106" s="2">
         <v>2</v>
       </c>
@@ -4008,7 +4008,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="107" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="107" spans="2:11">
       <c r="B107" s="2">
         <v>2</v>
       </c>
@@ -4040,7 +4040,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="108" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="108" spans="2:11">
       <c r="B108" s="2">
         <v>2</v>
       </c>
@@ -4072,7 +4072,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="109" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="109" spans="2:11">
       <c r="B109" s="2">
         <v>2</v>
       </c>
@@ -4104,7 +4104,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="110" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="110" spans="2:11">
       <c r="B110" s="2">
         <v>2</v>
       </c>
@@ -4136,7 +4136,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="111" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="111" spans="2:11">
       <c r="B111" s="2">
         <v>2</v>
       </c>
@@ -4168,7 +4168,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="112" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="112" spans="2:11">
       <c r="B112" s="2">
         <v>2</v>
       </c>
@@ -4200,7 +4200,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="113" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:11">
       <c r="B113" s="2">
         <v>2</v>
       </c>
@@ -4232,7 +4232,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="114" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="114" spans="2:11">
       <c r="B114" s="2">
         <v>2</v>
       </c>
@@ -4264,7 +4264,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="115" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="115" spans="2:11">
       <c r="B115" s="2">
         <v>3</v>
       </c>
@@ -4296,7 +4296,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="116" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="116" spans="2:11">
       <c r="B116" s="2">
         <v>3</v>
       </c>
@@ -4328,7 +4328,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="117" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="117" spans="2:11">
       <c r="B117" s="2">
         <v>3</v>
       </c>
@@ -4360,7 +4360,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="118" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="118" spans="2:11">
       <c r="B118" s="2">
         <v>3</v>
       </c>
@@ -4392,7 +4392,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="119" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="119" spans="2:11">
       <c r="B119" s="2">
         <v>3</v>
       </c>
@@ -4424,7 +4424,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="120" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="120" spans="2:11">
       <c r="B120" s="2">
         <v>3</v>
       </c>
@@ -4456,7 +4456,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="121" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="121" spans="2:11">
       <c r="B121" s="2">
         <v>3</v>
       </c>
@@ -4488,7 +4488,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="122" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="122" spans="2:11">
       <c r="B122" s="2">
         <v>3</v>
       </c>
@@ -4520,7 +4520,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="123" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="123" spans="2:11">
       <c r="B123" s="2">
         <v>3</v>
       </c>
@@ -4552,7 +4552,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="124" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="124" spans="2:11">
       <c r="B124" s="2">
         <v>3</v>
       </c>
@@ -4584,7 +4584,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="125" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="125" spans="2:11">
       <c r="B125" s="2">
         <v>3</v>
       </c>
@@ -4616,7 +4616,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="126" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="126" spans="2:11">
       <c r="B126" s="2">
         <v>3</v>
       </c>
@@ -4648,7 +4648,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="127" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="127" spans="2:11">
       <c r="B127" s="2">
         <v>3</v>
       </c>
@@ -4680,7 +4680,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="128" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="128" spans="2:11">
       <c r="B128" s="2">
         <v>3</v>
       </c>
@@ -4712,7 +4712,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="129" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="129" spans="2:11">
       <c r="B129" s="2">
         <v>3</v>
       </c>
@@ -4744,7 +4744,7 @@
         <v>12.743438154428157</v>
       </c>
     </row>
-    <row r="130" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="130" spans="2:11">
       <c r="B130" s="2">
         <v>3</v>
       </c>
@@ -4776,7 +4776,7 @@
         <v>13.11</v>
       </c>
     </row>
-    <row r="131" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="131" spans="2:11">
       <c r="B131" s="2">
         <v>3</v>
       </c>
@@ -4808,7 +4808,7 @@
         <v>12.097920581994543</v>
       </c>
     </row>
-    <row r="132" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="132" spans="2:11">
       <c r="B132" s="2">
         <v>3</v>
       </c>
@@ -4840,7 +4840,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="133" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="133" spans="2:11">
       <c r="B133" s="2">
         <v>3</v>
       </c>
@@ -4872,7 +4872,7 @@
         <v>13.549999999999999</v>
       </c>
     </row>
-    <row r="134" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="134" spans="2:11">
       <c r="B134" s="2">
         <v>3</v>
       </c>
@@ -4904,7 +4904,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="135" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="135" spans="2:11">
       <c r="B135" s="2">
         <v>3</v>
       </c>
@@ -4936,7 +4936,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="136" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="136" spans="2:11">
       <c r="B136" s="2">
         <v>3</v>
       </c>
@@ -4968,7 +4968,7 @@
         <v>13.560000000000002</v>
       </c>
     </row>
-    <row r="137" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="137" spans="2:11">
       <c r="B137" s="2">
         <v>3</v>
       </c>
@@ -5000,7 +5000,7 @@
         <v>13.14</v>
       </c>
     </row>
-    <row r="138" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="138" spans="2:11">
       <c r="B138" s="2">
         <v>3</v>
       </c>
@@ -5032,7 +5032,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="139" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="139" spans="2:11">
       <c r="B139" s="2">
         <v>3</v>
       </c>
@@ -5064,7 +5064,7 @@
         <v>13.343893899204247</v>
       </c>
     </row>
-    <row r="140" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="140" spans="2:11">
       <c r="B140" s="2">
         <v>3</v>
       </c>
@@ -5096,7 +5096,7 @@
         <v>13.799801123424928</v>
       </c>
     </row>
-    <row r="141" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="141" spans="2:11">
       <c r="B141" s="2">
         <v>3</v>
       </c>
@@ -5128,7 +5128,7 @@
         <v>13.929999999999998</v>
       </c>
     </row>
-    <row r="142" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="142" spans="2:11">
       <c r="B142" s="2">
         <v>3</v>
       </c>
@@ -5160,7 +5160,7 @@
         <v>13.26</v>
       </c>
     </row>
-    <row r="143" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="143" spans="2:11">
       <c r="B143" s="2">
         <v>4</v>
       </c>
@@ -5192,7 +5192,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="144" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="144" spans="2:11">
       <c r="B144" s="2">
         <v>4</v>
       </c>
@@ -5224,7 +5224,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="145" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="145" spans="2:11">
       <c r="B145" s="2">
         <v>4</v>
       </c>
@@ -5256,7 +5256,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="146" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="146" spans="2:11">
       <c r="B146" s="2">
         <v>4</v>
       </c>
@@ -5288,7 +5288,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="147" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="147" spans="2:11">
       <c r="B147" s="2">
         <v>4</v>
       </c>
@@ -5320,7 +5320,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="148" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="148" spans="2:11">
       <c r="B148" s="2">
         <v>4</v>
       </c>
@@ -5352,7 +5352,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="149" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="149" spans="2:11">
       <c r="B149" s="2">
         <v>4</v>
       </c>
@@ -5384,7 +5384,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="150" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="150" spans="2:11">
       <c r="B150" s="2">
         <v>4</v>
       </c>
@@ -5416,7 +5416,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="151" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="151" spans="2:11">
       <c r="B151" s="2">
         <v>4</v>
       </c>
@@ -5448,7 +5448,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="152" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="152" spans="2:11">
       <c r="B152" s="2">
         <v>4</v>
       </c>
@@ -5480,7 +5480,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="153" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="153" spans="2:11">
       <c r="B153" s="2">
         <v>4</v>
       </c>
@@ -5512,7 +5512,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="154" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="154" spans="2:11">
       <c r="B154" s="2">
         <v>4</v>
       </c>
@@ -5544,7 +5544,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="155" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="155" spans="2:11">
       <c r="B155" s="2">
         <v>4</v>
       </c>
@@ -5576,7 +5576,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="156" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="156" spans="2:11">
       <c r="B156" s="2">
         <v>4</v>
       </c>
@@ -5608,7 +5608,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="157" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="157" spans="2:11">
       <c r="B157" s="2">
         <v>4</v>
       </c>
@@ -5640,7 +5640,7 @@
         <v>13.089999999999998</v>
       </c>
     </row>
-    <row r="158" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="158" spans="2:11">
       <c r="B158" s="2">
         <v>4</v>
       </c>
@@ -5672,7 +5672,7 @@
         <v>13.380000000000003</v>
       </c>
     </row>
-    <row r="159" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="159" spans="2:11">
       <c r="B159" s="2">
         <v>4</v>
       </c>
@@ -5704,7 +5704,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="160" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="160" spans="2:11">
       <c r="B160" s="2">
         <v>4</v>
       </c>
@@ -5736,7 +5736,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="161" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="161" spans="2:11">
       <c r="B161" s="2">
         <v>4</v>
       </c>
@@ -5768,7 +5768,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="162" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="162" spans="2:11">
       <c r="B162" s="2">
         <v>4</v>
       </c>
@@ -5800,7 +5800,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="163" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="163" spans="2:11">
       <c r="B163" s="2">
         <v>4</v>
       </c>
@@ -5832,7 +5832,7 @@
         <v>13.550000000000002</v>
       </c>
     </row>
-    <row r="164" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="164" spans="2:11">
       <c r="B164" s="2">
         <v>4</v>
       </c>
@@ -5864,7 +5864,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="165" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="165" spans="2:11">
       <c r="B165" s="2">
         <v>4</v>
       </c>
@@ -5896,7 +5896,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="166" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="166" spans="2:11">
       <c r="B166" s="2">
         <v>4</v>
       </c>
@@ -5928,7 +5928,7 @@
         <v>13.455438105489774</v>
       </c>
     </row>
-    <row r="167" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="167" spans="2:11">
       <c r="B167" s="2">
         <v>4</v>
       </c>
@@ -5960,7 +5960,7 @@
         <v>13.838119469026548</v>
       </c>
     </row>
-    <row r="168" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="168" spans="2:11">
       <c r="B168" s="2">
         <v>4</v>
       </c>
@@ -5992,7 +5992,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="169" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="169" spans="2:11">
       <c r="B169" s="2">
         <v>4</v>
       </c>
@@ -6024,7 +6024,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="170" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="170" spans="2:11">
       <c r="B170" s="2">
         <v>4</v>
       </c>
@@ -6056,7 +6056,7 @@
         <v>13.690000000000001</v>
       </c>
     </row>
-    <row r="171" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="171" spans="2:11">
       <c r="B171" s="2">
         <v>1</v>
       </c>
@@ -6088,7 +6088,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="172" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="172" spans="2:11">
       <c r="B172" s="2">
         <v>1</v>
       </c>
@@ -6120,7 +6120,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="173" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="173" spans="2:11">
       <c r="B173" s="2">
         <v>1</v>
       </c>
@@ -6152,7 +6152,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="174" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="174" spans="2:11">
       <c r="B174" s="2">
         <v>1</v>
       </c>
@@ -6184,7 +6184,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="175" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="175" spans="2:11">
       <c r="B175" s="2">
         <v>1</v>
       </c>
@@ -6216,7 +6216,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="176" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="176" spans="2:11">
       <c r="B176" s="2">
         <v>1</v>
       </c>
@@ -6248,7 +6248,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="177" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="177" spans="2:11">
       <c r="B177" s="2">
         <v>1</v>
       </c>
@@ -6280,7 +6280,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="178" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="178" spans="2:11">
       <c r="B178" s="2">
         <v>1</v>
       </c>
@@ -6312,7 +6312,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="179" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="179" spans="2:11">
       <c r="B179" s="2">
         <v>1</v>
       </c>
@@ -6344,7 +6344,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="180" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="180" spans="2:11">
       <c r="B180" s="2">
         <v>1</v>
       </c>
@@ -6376,7 +6376,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="181" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="181" spans="2:11">
       <c r="B181" s="2">
         <v>1</v>
       </c>
@@ -6408,7 +6408,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="182" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="182" spans="2:11">
       <c r="B182" s="2">
         <v>1</v>
       </c>
@@ -6440,7 +6440,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="183" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="183" spans="2:11">
       <c r="B183" s="2">
         <v>1</v>
       </c>
@@ -6472,7 +6472,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="184" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="184" spans="2:11">
       <c r="B184" s="2">
         <v>1</v>
       </c>
@@ -6504,7 +6504,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="185" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="185" spans="2:11">
       <c r="B185" s="2">
         <v>2</v>
       </c>
@@ -6536,7 +6536,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="186" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="186" spans="2:11">
       <c r="B186" s="2">
         <v>2</v>
       </c>
@@ -6568,7 +6568,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="187" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="187" spans="2:11">
       <c r="B187" s="2">
         <v>2</v>
       </c>
@@ -6600,7 +6600,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="188" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="188" spans="2:11">
       <c r="B188" s="2">
         <v>2</v>
       </c>
@@ -6632,7 +6632,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="189" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="189" spans="2:11">
       <c r="B189" s="2">
         <v>2</v>
       </c>
@@ -6664,7 +6664,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="190" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="190" spans="2:11">
       <c r="B190" s="2">
         <v>2</v>
       </c>
@@ -6696,7 +6696,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="191" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="191" spans="2:11">
       <c r="B191" s="2">
         <v>2</v>
       </c>
@@ -6728,7 +6728,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="192" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="192" spans="2:11">
       <c r="B192" s="2">
         <v>2</v>
       </c>
@@ -6760,7 +6760,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="193" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="193" spans="2:11">
       <c r="B193" s="2">
         <v>2</v>
       </c>
@@ -6792,7 +6792,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="194" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="194" spans="2:11">
       <c r="B194" s="2">
         <v>2</v>
       </c>
@@ -6824,7 +6824,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="195" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="195" spans="2:11">
       <c r="B195" s="2">
         <v>2</v>
       </c>
@@ -6856,7 +6856,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="196" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="196" spans="2:11">
       <c r="B196" s="2">
         <v>2</v>
       </c>
@@ -6888,7 +6888,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="197" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="197" spans="2:11">
       <c r="B197" s="2">
         <v>2</v>
       </c>
@@ -6920,7 +6920,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="198" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="198" spans="2:11">
       <c r="B198" s="2">
         <v>2</v>
       </c>
@@ -6952,7 +6952,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="199" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="199" spans="2:11">
       <c r="B199" s="2">
         <v>3</v>
       </c>
@@ -6984,7 +6984,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="200" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="200" spans="2:11">
       <c r="B200" s="2">
         <v>3</v>
       </c>
@@ -7016,7 +7016,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="201" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="201" spans="2:11">
       <c r="B201" s="2">
         <v>3</v>
       </c>
@@ -7048,7 +7048,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="202" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="202" spans="2:11">
       <c r="B202" s="2">
         <v>3</v>
       </c>
@@ -7080,7 +7080,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="203" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="203" spans="2:11">
       <c r="B203" s="2">
         <v>3</v>
       </c>
@@ -7112,7 +7112,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="204" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="204" spans="2:11">
       <c r="B204" s="2">
         <v>3</v>
       </c>
@@ -7144,7 +7144,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="205" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="205" spans="2:11">
       <c r="B205" s="2">
         <v>3</v>
       </c>
@@ -7176,7 +7176,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="206" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="206" spans="2:11">
       <c r="B206" s="2">
         <v>3</v>
       </c>
@@ -7208,7 +7208,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="207" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="207" spans="2:11">
       <c r="B207" s="2">
         <v>3</v>
       </c>
@@ -7240,7 +7240,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="208" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="208" spans="2:11">
       <c r="B208" s="2">
         <v>3</v>
       </c>
@@ -7272,7 +7272,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="209" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="209" spans="2:11">
       <c r="B209" s="2">
         <v>3</v>
       </c>
@@ -7304,7 +7304,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="210" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="210" spans="2:11">
       <c r="B210" s="2">
         <v>3</v>
       </c>
@@ -7336,7 +7336,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="211" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="211" spans="2:11">
       <c r="B211" s="2">
         <v>3</v>
       </c>
@@ -7368,7 +7368,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="212" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="212" spans="2:11">
       <c r="B212" s="2">
         <v>3</v>
       </c>
@@ -7400,7 +7400,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="213" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="213" spans="2:11">
       <c r="B213" s="2">
         <v>3</v>
       </c>
@@ -7432,7 +7432,7 @@
         <v>13.133173681010607</v>
       </c>
     </row>
-    <row r="214" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="214" spans="2:11">
       <c r="B214" s="2">
         <v>3</v>
       </c>
@@ -7464,7 +7464,7 @@
         <v>13.54</v>
       </c>
     </row>
-    <row r="215" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="215" spans="2:11">
       <c r="B215" s="2">
         <v>3</v>
       </c>
@@ -7496,7 +7496,7 @@
         <v>12.461352935232899</v>
       </c>
     </row>
-    <row r="216" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="216" spans="2:11">
       <c r="B216" s="2">
         <v>3</v>
       </c>
@@ -7528,7 +7528,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="217" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="217" spans="2:11">
       <c r="B217" s="2">
         <v>3</v>
       </c>
@@ -7560,7 +7560,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="218" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="218" spans="2:11">
       <c r="B218" s="2">
         <v>3</v>
       </c>
@@ -7592,7 +7592,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="219" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="219" spans="2:11">
       <c r="B219" s="2">
         <v>3</v>
       </c>
@@ -7624,7 +7624,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="220" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="220" spans="2:11">
       <c r="B220" s="2">
         <v>3</v>
       </c>
@@ -7656,7 +7656,7 @@
         <v>13.920000000000002</v>
       </c>
     </row>
-    <row r="221" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="221" spans="2:11">
       <c r="B221" s="2">
         <v>3</v>
       </c>
@@ -7688,7 +7688,7 @@
         <v>13.55</v>
       </c>
     </row>
-    <row r="222" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="222" spans="2:11">
       <c r="B222" s="2">
         <v>3</v>
       </c>
@@ -7720,7 +7720,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="223" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="223" spans="2:11">
       <c r="B223" s="2">
         <v>3</v>
       </c>
@@ -7752,7 +7752,7 @@
         <v>13.839584438549954</v>
       </c>
     </row>
-    <row r="224" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="224" spans="2:11">
       <c r="B224" s="2">
         <v>3</v>
       </c>
@@ -7784,7 +7784,7 @@
         <v>14.364701685137391</v>
       </c>
     </row>
-    <row r="225" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="225" spans="2:11">
       <c r="B225" s="2">
         <v>3</v>
       </c>
@@ -7816,7 +7816,7 @@
         <v>14.43</v>
       </c>
     </row>
-    <row r="226" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="226" spans="2:11">
       <c r="B226" s="2">
         <v>3</v>
       </c>
@@ -7848,7 +7848,7 @@
         <v>13.699999999999998</v>
       </c>
     </row>
-    <row r="227" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="227" spans="2:11">
       <c r="B227" s="2">
         <v>4</v>
       </c>
@@ -7880,7 +7880,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="228" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="228" spans="2:11">
       <c r="B228" s="2">
         <v>4</v>
       </c>
@@ -7912,7 +7912,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="229" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="229" spans="2:11">
       <c r="B229" s="2">
         <v>4</v>
       </c>
@@ -7944,7 +7944,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="230" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="230" spans="2:11">
       <c r="B230" s="2">
         <v>4</v>
       </c>
@@ -7976,7 +7976,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="231" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="231" spans="2:11">
       <c r="B231" s="2">
         <v>4</v>
       </c>
@@ -8008,7 +8008,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="232" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="232" spans="2:11">
       <c r="B232" s="2">
         <v>4</v>
       </c>
@@ -8040,7 +8040,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="233" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="233" spans="2:11">
       <c r="B233" s="2">
         <v>4</v>
       </c>
@@ -8072,7 +8072,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="234" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="234" spans="2:11">
       <c r="B234" s="2">
         <v>4</v>
       </c>
@@ -8104,7 +8104,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="235" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="235" spans="2:11">
       <c r="B235" s="2">
         <v>4</v>
       </c>
@@ -8136,7 +8136,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="236" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="236" spans="2:11">
       <c r="B236" s="2">
         <v>4</v>
       </c>
@@ -8168,7 +8168,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="237" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="237" spans="2:11">
       <c r="B237" s="2">
         <v>4</v>
       </c>
@@ -8200,7 +8200,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="238" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="238" spans="2:11">
       <c r="B238" s="2">
         <v>4</v>
       </c>
@@ -8232,7 +8232,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="239" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="239" spans="2:11">
       <c r="B239" s="2">
         <v>4</v>
       </c>
@@ -8264,7 +8264,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="240" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="240" spans="2:11">
       <c r="B240" s="2">
         <v>4</v>
       </c>
@@ -8296,7 +8296,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="241" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="241" spans="2:11">
       <c r="B241" s="2">
         <v>4</v>
       </c>
@@ -8328,7 +8328,7 @@
         <v>13.49</v>
       </c>
     </row>
-    <row r="242" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="242" spans="2:11">
       <c r="B242" s="2">
         <v>4</v>
       </c>
@@ -8360,7 +8360,7 @@
         <v>13.83</v>
       </c>
     </row>
-    <row r="243" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="243" spans="2:11">
       <c r="B243" s="2">
         <v>4</v>
       </c>
@@ -8392,7 +8392,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="244" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="244" spans="2:11">
       <c r="B244" s="2">
         <v>4</v>
       </c>
@@ -8424,7 +8424,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="245" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="245" spans="2:11">
       <c r="B245" s="2">
         <v>4</v>
       </c>
@@ -8456,7 +8456,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="246" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="246" spans="2:11">
       <c r="B246" s="2">
         <v>4</v>
       </c>
@@ -8488,7 +8488,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="247" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="247" spans="2:11">
       <c r="B247" s="2">
         <v>4</v>
       </c>
@@ -8520,7 +8520,7 @@
         <v>14.02</v>
       </c>
     </row>
-    <row r="248" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="248" spans="2:11">
       <c r="B248" s="2">
         <v>4</v>
       </c>
@@ -8552,7 +8552,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="249" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="249" spans="2:11">
       <c r="B249" s="2">
         <v>4</v>
       </c>
@@ -8584,7 +8584,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="250" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="250" spans="2:11">
       <c r="B250" s="2">
         <v>4</v>
       </c>
@@ -8616,7 +8616,7 @@
         <v>13.898170075349839</v>
       </c>
     </row>
-    <row r="251" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="251" spans="2:11">
       <c r="B251" s="2">
         <v>4</v>
       </c>
@@ -8648,7 +8648,7 @@
         <v>14.328119469026548</v>
       </c>
     </row>
-    <row r="252" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="252" spans="2:11">
       <c r="B252" s="2">
         <v>4</v>
       </c>
@@ -8680,7 +8680,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="253" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="253" spans="2:11">
       <c r="B253" s="2">
         <v>4</v>
       </c>
@@ -8712,7 +8712,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="254" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="254" spans="2:11">
       <c r="B254" s="2">
         <v>4</v>
       </c>
@@ -8744,7 +8744,7 @@
         <v>14.12</v>
       </c>
     </row>
-    <row r="255" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="255" spans="2:11">
       <c r="B255" s="2">
         <v>1</v>
       </c>
@@ -8776,7 +8776,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="256" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="256" spans="2:11">
       <c r="B256" s="2">
         <v>1</v>
       </c>
@@ -8808,7 +8808,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="257" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="257" spans="2:11">
       <c r="B257" s="2">
         <v>1</v>
       </c>
@@ -8840,7 +8840,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="258" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="258" spans="2:11">
       <c r="B258" s="2">
         <v>1</v>
       </c>
@@ -8872,7 +8872,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="259" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="259" spans="2:11">
       <c r="B259" s="2">
         <v>1</v>
       </c>
@@ -8904,7 +8904,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="260" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="260" spans="2:11">
       <c r="B260" s="2">
         <v>1</v>
       </c>
@@ -8936,7 +8936,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="261" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="261" spans="2:11">
       <c r="B261" s="2">
         <v>1</v>
       </c>
@@ -8968,7 +8968,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="262" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="262" spans="2:11">
       <c r="B262" s="2">
         <v>1</v>
       </c>
@@ -9000,7 +9000,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="263" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="263" spans="2:11">
       <c r="B263" s="2">
         <v>1</v>
       </c>
@@ -9032,7 +9032,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="264" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="264" spans="2:11">
       <c r="B264" s="2">
         <v>1</v>
       </c>
@@ -9064,7 +9064,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="265" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="265" spans="2:11">
       <c r="B265" s="2">
         <v>1</v>
       </c>
@@ -9096,7 +9096,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="266" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="266" spans="2:11">
       <c r="B266" s="2">
         <v>1</v>
       </c>
@@ -9128,7 +9128,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="267" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="267" spans="2:11">
       <c r="B267" s="2">
         <v>1</v>
       </c>
@@ -9160,7 +9160,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="268" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="268" spans="2:11">
       <c r="B268" s="2">
         <v>1</v>
       </c>
@@ -9192,7 +9192,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="269" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="269" spans="2:11">
       <c r="B269" s="2">
         <v>2</v>
       </c>
@@ -9224,7 +9224,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="270" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="270" spans="2:11">
       <c r="B270" s="2">
         <v>2</v>
       </c>
@@ -9256,7 +9256,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="271" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="271" spans="2:11">
       <c r="B271" s="2">
         <v>2</v>
       </c>
@@ -9288,7 +9288,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="272" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="272" spans="2:11">
       <c r="B272" s="2">
         <v>2</v>
       </c>
@@ -9320,7 +9320,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="273" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="273" spans="2:11">
       <c r="B273" s="2">
         <v>2</v>
       </c>
@@ -9352,7 +9352,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="274" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="274" spans="2:11">
       <c r="B274" s="2">
         <v>2</v>
       </c>
@@ -9384,7 +9384,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="275" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="275" spans="2:11">
       <c r="B275" s="2">
         <v>2</v>
       </c>
@@ -9416,7 +9416,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="276" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="276" spans="2:11">
       <c r="B276" s="2">
         <v>2</v>
       </c>
@@ -9448,7 +9448,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="277" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="277" spans="2:11">
       <c r="B277" s="2">
         <v>2</v>
       </c>
@@ -9480,7 +9480,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="278" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="278" spans="2:11">
       <c r="B278" s="2">
         <v>2</v>
       </c>
@@ -9512,7 +9512,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="279" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="279" spans="2:11">
       <c r="B279" s="2">
         <v>2</v>
       </c>
@@ -9544,7 +9544,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="280" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="280" spans="2:11">
       <c r="B280" s="2">
         <v>2</v>
       </c>
@@ -9576,7 +9576,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="281" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="281" spans="2:11">
       <c r="B281" s="2">
         <v>2</v>
       </c>
@@ -9608,7 +9608,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="282" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="282" spans="2:11">
       <c r="B282" s="2">
         <v>2</v>
       </c>
@@ -9640,7 +9640,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="283" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="283" spans="2:11">
       <c r="B283" s="2">
         <v>3</v>
       </c>
@@ -9672,7 +9672,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="284" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="284" spans="2:11">
       <c r="B284" s="2">
         <v>3</v>
       </c>
@@ -9704,7 +9704,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="285" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="285" spans="2:11">
       <c r="B285" s="2">
         <v>3</v>
       </c>
@@ -9736,7 +9736,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="286" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="286" spans="2:11">
       <c r="B286" s="2">
         <v>3</v>
       </c>
@@ -9768,7 +9768,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="287" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="287" spans="2:11">
       <c r="B287" s="2">
         <v>3</v>
       </c>
@@ -9800,7 +9800,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="288" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="288" spans="2:11">
       <c r="B288" s="2">
         <v>3</v>
       </c>
@@ -9832,7 +9832,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="289" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="289" spans="2:11">
       <c r="B289" s="2">
         <v>3</v>
       </c>
@@ -9864,7 +9864,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="290" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="290" spans="2:11">
       <c r="B290" s="2">
         <v>3</v>
       </c>
@@ -9896,7 +9896,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="291" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="291" spans="2:11">
       <c r="B291" s="2">
         <v>3</v>
       </c>
@@ -9928,7 +9928,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="292" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="292" spans="2:11">
       <c r="B292" s="2">
         <v>3</v>
       </c>
@@ -9960,7 +9960,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="293" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="293" spans="2:11">
       <c r="B293" s="2">
         <v>3</v>
       </c>
@@ -9992,7 +9992,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="294" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="294" spans="2:11">
       <c r="B294" s="2">
         <v>3</v>
       </c>
@@ -10024,7 +10024,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="295" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="295" spans="2:11">
       <c r="B295" s="2">
         <v>3</v>
       </c>
@@ -10056,7 +10056,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="296" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="296" spans="2:11">
       <c r="B296" s="2">
         <v>3</v>
       </c>
@@ -10088,7 +10088,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="297" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="297" spans="2:11">
       <c r="B297" s="2">
         <v>3</v>
       </c>
@@ -10120,7 +10120,7 @@
         <v>12.963702627845706</v>
       </c>
     </row>
-    <row r="298" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="298" spans="2:11">
       <c r="B298" s="2">
         <v>3</v>
       </c>
@@ -10152,7 +10152,7 @@
         <v>13.249999999999998</v>
       </c>
     </row>
-    <row r="299" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="299" spans="2:11">
       <c r="B299" s="2">
         <v>3</v>
       </c>
@@ -10184,7 +10184,7 @@
         <v>12.32448822875619</v>
       </c>
     </row>
-    <row r="300" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="300" spans="2:11">
       <c r="B300" s="2">
         <v>3</v>
       </c>
@@ -10216,7 +10216,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="301" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="301" spans="2:11">
       <c r="B301" s="2">
         <v>3</v>
       </c>
@@ -10248,7 +10248,7 @@
         <v>13.7</v>
       </c>
     </row>
-    <row r="302" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="302" spans="2:11">
       <c r="B302" s="2">
         <v>3</v>
       </c>
@@ -10280,7 +10280,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="303" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="303" spans="2:11">
       <c r="B303" s="2">
         <v>3</v>
       </c>
@@ -10312,7 +10312,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="304" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="304" spans="2:11">
       <c r="B304" s="2">
         <v>3</v>
       </c>
@@ -10344,7 +10344,7 @@
         <v>14.230000000000002</v>
       </c>
     </row>
-    <row r="305" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="305" spans="2:11">
       <c r="B305" s="2">
         <v>3</v>
       </c>
@@ -10376,7 +10376,7 @@
         <v>13.269999999999998</v>
       </c>
     </row>
-    <row r="306" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="306" spans="2:11">
       <c r="B306" s="2">
         <v>3</v>
       </c>
@@ -10408,7 +10408,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="307" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="307" spans="2:11">
       <c r="B307" s="2">
         <v>3</v>
       </c>
@@ -10440,7 +10440,7 @@
         <v>13.438203359858536</v>
       </c>
     </row>
-    <row r="308" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="308" spans="2:11">
       <c r="B308" s="2">
         <v>3</v>
       </c>
@@ -10472,7 +10472,7 @@
         <v>13.860198876575073</v>
       </c>
     </row>
-    <row r="309" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="309" spans="2:11">
       <c r="B309" s="2">
         <v>3</v>
       </c>
@@ -10504,7 +10504,7 @@
         <v>14.07</v>
       </c>
     </row>
-    <row r="310" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="310" spans="2:11">
       <c r="B310" s="2">
         <v>3</v>
       </c>
@@ -10536,7 +10536,7 @@
         <v>13.31</v>
       </c>
     </row>
-    <row r="311" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="311" spans="2:11">
       <c r="B311" s="2">
         <v>4</v>
       </c>
@@ -10568,7 +10568,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="312" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="312" spans="2:11">
       <c r="B312" s="2">
         <v>4</v>
       </c>
@@ -10600,7 +10600,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="313" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="313" spans="2:11">
       <c r="B313" s="2">
         <v>4</v>
       </c>
@@ -10632,7 +10632,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="314" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="314" spans="2:11">
       <c r="B314" s="2">
         <v>4</v>
       </c>
@@ -10664,7 +10664,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="315" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="315" spans="2:11">
       <c r="B315" s="2">
         <v>4</v>
       </c>
@@ -10696,7 +10696,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="316" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="316" spans="2:11">
       <c r="B316" s="2">
         <v>4</v>
       </c>
@@ -10728,7 +10728,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="317" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="317" spans="2:11">
       <c r="B317" s="2">
         <v>4</v>
       </c>
@@ -10760,7 +10760,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="318" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="318" spans="2:11">
       <c r="B318" s="2">
         <v>4</v>
       </c>
@@ -10792,7 +10792,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="319" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="319" spans="2:11">
       <c r="B319" s="2">
         <v>4</v>
       </c>
@@ -10824,7 +10824,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="320" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="320" spans="2:11">
       <c r="B320" s="2">
         <v>4</v>
       </c>
@@ -10856,7 +10856,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="321" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="321" spans="2:11">
       <c r="B321" s="2">
         <v>4</v>
       </c>
@@ -10888,7 +10888,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="322" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="322" spans="2:11">
       <c r="B322" s="2">
         <v>4</v>
       </c>
@@ -10920,7 +10920,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="323" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="323" spans="2:11">
       <c r="B323" s="2">
         <v>4</v>
       </c>
@@ -10952,7 +10952,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="324" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="324" spans="2:11">
       <c r="B324" s="2">
         <v>4</v>
       </c>
@@ -10984,7 +10984,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="325" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="325" spans="2:11">
       <c r="B325" s="2">
         <v>4</v>
       </c>
@@ -11016,7 +11016,7 @@
         <v>13.240000000000002</v>
       </c>
     </row>
-    <row r="326" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="326" spans="2:11">
       <c r="B326" s="2">
         <v>4</v>
       </c>
@@ -11048,7 +11048,7 @@
         <v>13.459999999999999</v>
       </c>
     </row>
-    <row r="327" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="327" spans="2:11">
       <c r="B327" s="2">
         <v>4</v>
       </c>
@@ -11080,7 +11080,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="328" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="328" spans="2:11">
       <c r="B328" s="2">
         <v>4</v>
       </c>
@@ -11112,7 +11112,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="329" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="329" spans="2:11">
       <c r="B329" s="2">
         <v>4</v>
       </c>
@@ -11144,7 +11144,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="330" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="330" spans="2:11">
       <c r="B330" s="2">
         <v>4</v>
       </c>
@@ -11176,7 +11176,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="331" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="331" spans="2:11">
       <c r="B331" s="2">
         <v>4</v>
       </c>
@@ -11208,7 +11208,7 @@
         <v>13.68</v>
       </c>
     </row>
-    <row r="332" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="332" spans="2:11">
       <c r="B332" s="2">
         <v>4</v>
       </c>
@@ -11240,7 +11240,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="333" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="333" spans="2:11">
       <c r="B333" s="2">
         <v>4</v>
       </c>
@@ -11272,7 +11272,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="334" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="334" spans="2:11">
       <c r="B334" s="2">
         <v>4</v>
       </c>
@@ -11304,7 +11304,7 @@
         <v>13.56724219590958</v>
       </c>
     </row>
-    <row r="335" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="335" spans="2:11">
       <c r="B335" s="2">
         <v>4</v>
       </c>
@@ -11336,7 +11336,7 @@
         <v>13.996194690265485</v>
       </c>
     </row>
-    <row r="336" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="336" spans="2:11">
       <c r="B336" s="2">
         <v>4</v>
       </c>
@@ -11368,7 +11368,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="337" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="337" spans="2:11">
       <c r="B337" s="2">
         <v>4</v>
       </c>
@@ -11400,7 +11400,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="338" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="338" spans="2:11">
       <c r="B338" s="2">
         <v>4</v>
       </c>
@@ -11432,7 +11432,7 @@
         <v>13.77</v>
       </c>
     </row>
-    <row r="339" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="339" spans="2:11">
       <c r="B339" s="2">
         <v>1</v>
       </c>
@@ -11464,7 +11464,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="340" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="340" spans="2:11">
       <c r="B340" s="2">
         <v>1</v>
       </c>
@@ -11496,7 +11496,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="341" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="341" spans="2:11">
       <c r="B341" s="2">
         <v>1</v>
       </c>
@@ -11528,7 +11528,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="342" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="342" spans="2:11">
       <c r="B342" s="2">
         <v>1</v>
       </c>
@@ -11560,7 +11560,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="343" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="343" spans="2:11">
       <c r="B343" s="2">
         <v>1</v>
       </c>
@@ -11592,7 +11592,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="344" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="344" spans="2:11">
       <c r="B344" s="2">
         <v>1</v>
       </c>
@@ -11624,7 +11624,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="345" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="345" spans="2:11">
       <c r="B345" s="2">
         <v>1</v>
       </c>
@@ -11656,7 +11656,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="346" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="346" spans="2:11">
       <c r="B346" s="2">
         <v>1</v>
       </c>
@@ -11688,7 +11688,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="347" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="347" spans="2:11">
       <c r="B347" s="2">
         <v>1</v>
       </c>
@@ -11720,7 +11720,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="348" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="348" spans="2:11">
       <c r="B348" s="2">
         <v>1</v>
       </c>
@@ -11752,7 +11752,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="349" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="349" spans="2:11">
       <c r="B349" s="2">
         <v>1</v>
       </c>
@@ -11784,7 +11784,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="350" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="350" spans="2:11">
       <c r="B350" s="2">
         <v>1</v>
       </c>
@@ -11816,7 +11816,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="351" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="351" spans="2:11">
       <c r="B351" s="2">
         <v>1</v>
       </c>
@@ -11848,7 +11848,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="352" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="352" spans="2:11">
       <c r="B352" s="2">
         <v>1</v>
       </c>
@@ -11880,7 +11880,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="353" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="353" spans="2:11">
       <c r="B353" s="2">
         <v>2</v>
       </c>
@@ -11912,7 +11912,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="354" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="354" spans="2:11">
       <c r="B354" s="2">
         <v>2</v>
       </c>
@@ -11944,7 +11944,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="355" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="355" spans="2:11">
       <c r="B355" s="2">
         <v>2</v>
       </c>
@@ -11976,7 +11976,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="356" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="356" spans="2:11">
       <c r="B356" s="2">
         <v>2</v>
       </c>
@@ -12008,7 +12008,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="357" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="357" spans="2:11">
       <c r="B357" s="2">
         <v>2</v>
       </c>
@@ -12040,7 +12040,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="358" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="358" spans="2:11">
       <c r="B358" s="2">
         <v>2</v>
       </c>
@@ -12072,7 +12072,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="359" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="359" spans="2:11">
       <c r="B359" s="2">
         <v>2</v>
       </c>
@@ -12104,7 +12104,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="360" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="360" spans="2:11">
       <c r="B360" s="2">
         <v>2</v>
       </c>
@@ -12136,7 +12136,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="361" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="361" spans="2:11">
       <c r="B361" s="2">
         <v>2</v>
       </c>
@@ -12168,7 +12168,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="362" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="362" spans="2:11">
       <c r="B362" s="2">
         <v>2</v>
       </c>
@@ -12200,7 +12200,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="363" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="363" spans="2:11">
       <c r="B363" s="2">
         <v>2</v>
       </c>
@@ -12232,7 +12232,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="364" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="364" spans="2:11">
       <c r="B364" s="2">
         <v>2</v>
       </c>
@@ -12264,7 +12264,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="365" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="365" spans="2:11">
       <c r="B365" s="2">
         <v>2</v>
       </c>
@@ -12296,7 +12296,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="366" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="366" spans="2:11">
       <c r="B366" s="2">
         <v>2</v>
       </c>
@@ -12328,7 +12328,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="367" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="367" spans="2:11">
       <c r="B367" s="2">
         <v>3</v>
       </c>
@@ -12360,7 +12360,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="368" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="368" spans="2:11">
       <c r="B368" s="2">
         <v>3</v>
       </c>
@@ -12392,7 +12392,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="369" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="369" spans="2:11">
       <c r="B369" s="2">
         <v>3</v>
       </c>
@@ -12424,7 +12424,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="370" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="370" spans="2:11">
       <c r="B370" s="2">
         <v>3</v>
       </c>
@@ -12456,7 +12456,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="371" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="371" spans="2:11">
       <c r="B371" s="2">
         <v>3</v>
       </c>
@@ -12488,7 +12488,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="372" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="372" spans="2:11">
       <c r="B372" s="2">
         <v>3</v>
       </c>
@@ -12520,7 +12520,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="373" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="373" spans="2:11">
       <c r="B373" s="2">
         <v>3</v>
       </c>
@@ -12552,7 +12552,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="374" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="374" spans="2:11">
       <c r="B374" s="2">
         <v>3</v>
       </c>
@@ -12584,7 +12584,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="375" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="375" spans="2:11">
       <c r="B375" s="2">
         <v>3</v>
       </c>
@@ -12616,7 +12616,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="376" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="376" spans="2:11">
       <c r="B376" s="2">
         <v>3</v>
       </c>
@@ -12648,7 +12648,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="377" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="377" spans="2:11">
       <c r="B377" s="2">
         <v>3</v>
       </c>
@@ -12680,7 +12680,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="378" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="378" spans="2:11">
       <c r="B378" s="2">
         <v>3</v>
       </c>
@@ -12712,7 +12712,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="379" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="379" spans="2:11">
       <c r="B379" s="2">
         <v>3</v>
       </c>
@@ -12744,7 +12744,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="380" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="380" spans="2:11">
       <c r="B380" s="2">
         <v>3</v>
       </c>
@@ -12776,7 +12776,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="381" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="381" spans="2:11">
       <c r="B381" s="2">
         <v>3</v>
       </c>
@@ -12808,7 +12808,7 @@
         <v>12.843438154428156</v>
       </c>
     </row>
-    <row r="382" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="382" spans="2:11">
       <c r="B382" s="2">
         <v>3</v>
       </c>
@@ -12840,7 +12840,7 @@
         <v>13.209999999999999</v>
       </c>
     </row>
-    <row r="383" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="383" spans="2:11">
       <c r="B383" s="2">
         <v>3</v>
       </c>
@@ -12872,7 +12872,7 @@
         <v>12.197920581994543</v>
       </c>
     </row>
-    <row r="384" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="384" spans="2:11">
       <c r="B384" s="2">
         <v>3</v>
       </c>
@@ -12904,7 +12904,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="385" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="385" spans="2:11">
       <c r="B385" s="2">
         <v>3</v>
       </c>
@@ -12936,7 +12936,7 @@
         <v>13.649999999999999</v>
       </c>
     </row>
-    <row r="386" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="386" spans="2:11">
       <c r="B386" s="2">
         <v>3</v>
       </c>
@@ -12968,7 +12968,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="387" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="387" spans="2:11">
       <c r="B387" s="2">
         <v>3</v>
       </c>
@@ -13000,7 +13000,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="388" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="388" spans="2:11">
       <c r="B388" s="2">
         <v>3</v>
       </c>
@@ -13032,7 +13032,7 @@
         <v>13.660000000000002</v>
       </c>
     </row>
-    <row r="389" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="389" spans="2:11">
       <c r="B389" s="2">
         <v>3</v>
       </c>
@@ -13064,7 +13064,7 @@
         <v>13.24</v>
       </c>
     </row>
-    <row r="390" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="390" spans="2:11">
       <c r="B390" s="2">
         <v>3</v>
       </c>
@@ -13096,7 +13096,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="391" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="391" spans="2:11">
       <c r="B391" s="2">
         <v>3</v>
       </c>
@@ -13128,7 +13128,7 @@
         <v>13.443893899204246</v>
       </c>
     </row>
-    <row r="392" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="392" spans="2:11">
       <c r="B392" s="2">
         <v>3</v>
       </c>
@@ -13160,7 +13160,7 @@
         <v>13.899801123424927</v>
       </c>
     </row>
-    <row r="393" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="393" spans="2:11">
       <c r="B393" s="2">
         <v>3</v>
       </c>
@@ -13192,7 +13192,7 @@
         <v>14.029999999999998</v>
       </c>
     </row>
-    <row r="394" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="394" spans="2:11">
       <c r="B394" s="2">
         <v>3</v>
       </c>
@@ -13224,7 +13224,7 @@
         <v>13.36</v>
       </c>
     </row>
-    <row r="395" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="395" spans="2:11">
       <c r="B395" s="2">
         <v>4</v>
       </c>
@@ -13256,7 +13256,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="396" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="396" spans="2:11">
       <c r="B396" s="2">
         <v>4</v>
       </c>
@@ -13288,7 +13288,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="397" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="397" spans="2:11">
       <c r="B397" s="2">
         <v>4</v>
       </c>
@@ -13320,7 +13320,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="398" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="398" spans="2:11">
       <c r="B398" s="2">
         <v>4</v>
       </c>
@@ -13352,7 +13352,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="399" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="399" spans="2:11">
       <c r="B399" s="2">
         <v>4</v>
       </c>
@@ -13384,7 +13384,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="400" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="400" spans="2:11">
       <c r="B400" s="2">
         <v>4</v>
       </c>
@@ -13416,7 +13416,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="401" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="401" spans="2:11">
       <c r="B401" s="2">
         <v>4</v>
       </c>
@@ -13448,7 +13448,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="402" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="402" spans="2:11">
       <c r="B402" s="2">
         <v>4</v>
       </c>
@@ -13480,7 +13480,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="403" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="403" spans="2:11">
       <c r="B403" s="2">
         <v>4</v>
       </c>
@@ -13512,7 +13512,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="404" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="404" spans="2:11">
       <c r="B404" s="2">
         <v>4</v>
       </c>
@@ -13544,7 +13544,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="405" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="405" spans="2:11">
       <c r="B405" s="2">
         <v>4</v>
       </c>
@@ -13576,7 +13576,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="406" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="406" spans="2:11">
       <c r="B406" s="2">
         <v>4</v>
       </c>
@@ -13608,7 +13608,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="407" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="407" spans="2:11">
       <c r="B407" s="2">
         <v>4</v>
       </c>
@@ -13640,7 +13640,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="408" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="408" spans="2:11">
       <c r="B408" s="2">
         <v>4</v>
       </c>
@@ -13672,7 +13672,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="409" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="409" spans="2:11">
       <c r="B409" s="2">
         <v>4</v>
       </c>
@@ -13704,7 +13704,7 @@
         <v>13.189999999999998</v>
       </c>
     </row>
-    <row r="410" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="410" spans="2:11">
       <c r="B410" s="2">
         <v>4</v>
       </c>
@@ -13736,7 +13736,7 @@
         <v>13.480000000000002</v>
       </c>
     </row>
-    <row r="411" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="411" spans="2:11">
       <c r="B411" s="2">
         <v>4</v>
       </c>
@@ -13768,7 +13768,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="412" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="412" spans="2:11">
       <c r="B412" s="2">
         <v>4</v>
       </c>
@@ -13800,7 +13800,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="413" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="413" spans="2:11">
       <c r="B413" s="2">
         <v>4</v>
       </c>
@@ -13832,7 +13832,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="414" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="414" spans="2:11">
       <c r="B414" s="2">
         <v>4</v>
       </c>
@@ -13864,7 +13864,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="415" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="415" spans="2:11">
       <c r="B415" s="2">
         <v>4</v>
       </c>
@@ -13896,7 +13896,7 @@
         <v>13.650000000000002</v>
       </c>
     </row>
-    <row r="416" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="416" spans="2:11">
       <c r="B416" s="2">
         <v>4</v>
       </c>
@@ -13928,7 +13928,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="417" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="417" spans="2:11">
       <c r="B417" s="2">
         <v>4</v>
       </c>
@@ -13960,7 +13960,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="418" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="418" spans="2:11">
       <c r="B418" s="2">
         <v>4</v>
       </c>
@@ -13992,7 +13992,7 @@
         <v>13.555438105489774</v>
       </c>
     </row>
-    <row r="419" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="419" spans="2:11">
       <c r="B419" s="2">
         <v>4</v>
       </c>
@@ -14024,7 +14024,7 @@
         <v>13.938119469026548</v>
       </c>
     </row>
-    <row r="420" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="420" spans="2:11">
       <c r="B420" s="2">
         <v>4</v>
       </c>
@@ -14056,7 +14056,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="421" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="421" spans="2:11">
       <c r="B421" s="2">
         <v>4</v>
       </c>
@@ -14088,7 +14088,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="422" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="422" spans="2:11">
       <c r="B422" s="2">
         <v>4</v>
       </c>
@@ -14120,7 +14120,7 @@
         <v>13.790000000000001</v>
       </c>
     </row>
-    <row r="423" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="423" spans="2:11">
       <c r="B423" s="2">
         <v>1</v>
       </c>
@@ -14152,7 +14152,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="424" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="424" spans="2:11">
       <c r="B424" s="2">
         <v>1</v>
       </c>
@@ -14184,7 +14184,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="425" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="425" spans="2:11">
       <c r="B425" s="2">
         <v>1</v>
       </c>
@@ -14216,7 +14216,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="426" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="426" spans="2:11">
       <c r="B426" s="2">
         <v>1</v>
       </c>
@@ -14248,7 +14248,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="427" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="427" spans="2:11">
       <c r="B427" s="2">
         <v>1</v>
       </c>
@@ -14280,7 +14280,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="428" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="428" spans="2:11">
       <c r="B428" s="2">
         <v>1</v>
       </c>
@@ -14312,7 +14312,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="429" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="429" spans="2:11">
       <c r="B429" s="2">
         <v>1</v>
       </c>
@@ -14344,7 +14344,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="430" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="430" spans="2:11">
       <c r="B430" s="2">
         <v>1</v>
       </c>
@@ -14376,7 +14376,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="431" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="431" spans="2:11">
       <c r="B431" s="2">
         <v>1</v>
       </c>
@@ -14408,7 +14408,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="432" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="432" spans="2:11">
       <c r="B432" s="2">
         <v>1</v>
       </c>
@@ -14440,7 +14440,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="433" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="433" spans="2:11">
       <c r="B433" s="2">
         <v>1</v>
       </c>
@@ -14472,7 +14472,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="434" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="434" spans="2:11">
       <c r="B434" s="2">
         <v>1</v>
       </c>
@@ -14504,7 +14504,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="435" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="435" spans="2:11">
       <c r="B435" s="2">
         <v>1</v>
       </c>
@@ -14536,7 +14536,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="436" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="436" spans="2:11">
       <c r="B436" s="2">
         <v>1</v>
       </c>
@@ -14568,7 +14568,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="437" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="437" spans="2:11">
       <c r="B437" s="2">
         <v>2</v>
       </c>
@@ -14600,7 +14600,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="438" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="438" spans="2:11">
       <c r="B438" s="2">
         <v>2</v>
       </c>
@@ -14632,7 +14632,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="439" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="439" spans="2:11">
       <c r="B439" s="2">
         <v>2</v>
       </c>
@@ -14664,7 +14664,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="440" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="440" spans="2:11">
       <c r="B440" s="2">
         <v>2</v>
       </c>
@@ -14696,7 +14696,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="441" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="441" spans="2:11">
       <c r="B441" s="2">
         <v>2</v>
       </c>
@@ -14728,7 +14728,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="442" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="442" spans="2:11">
       <c r="B442" s="2">
         <v>2</v>
       </c>
@@ -14760,7 +14760,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="443" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="443" spans="2:11">
       <c r="B443" s="2">
         <v>2</v>
       </c>
@@ -14792,7 +14792,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="444" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="444" spans="2:11">
       <c r="B444" s="2">
         <v>2</v>
       </c>
@@ -14824,7 +14824,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="445" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="445" spans="2:11">
       <c r="B445" s="2">
         <v>2</v>
       </c>
@@ -14856,7 +14856,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="446" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="446" spans="2:11">
       <c r="B446" s="2">
         <v>2</v>
       </c>
@@ -14888,7 +14888,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="447" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="447" spans="2:11">
       <c r="B447" s="2">
         <v>2</v>
       </c>
@@ -14920,7 +14920,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="448" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="448" spans="2:11">
       <c r="B448" s="2">
         <v>2</v>
       </c>
@@ -14952,7 +14952,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="449" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="449" spans="2:11">
       <c r="B449" s="2">
         <v>2</v>
       </c>
@@ -14984,7 +14984,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="450" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="450" spans="2:11">
       <c r="B450" s="2">
         <v>2</v>
       </c>
@@ -15016,7 +15016,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="451" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="451" spans="2:11">
       <c r="B451" s="2">
         <v>3</v>
       </c>
@@ -15048,7 +15048,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="452" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="452" spans="2:11">
       <c r="B452" s="2">
         <v>3</v>
       </c>
@@ -15080,7 +15080,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="453" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="453" spans="2:11">
       <c r="B453" s="2">
         <v>3</v>
       </c>
@@ -15112,7 +15112,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="454" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="454" spans="2:11">
       <c r="B454" s="2">
         <v>3</v>
       </c>
@@ -15144,7 +15144,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="455" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="455" spans="2:11">
       <c r="B455" s="2">
         <v>3</v>
       </c>
@@ -15176,7 +15176,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="456" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="456" spans="2:11">
       <c r="B456" s="2">
         <v>3</v>
       </c>
@@ -15208,7 +15208,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="457" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="457" spans="2:11">
       <c r="B457" s="2">
         <v>3</v>
       </c>
@@ -15240,7 +15240,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="458" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="458" spans="2:11">
       <c r="B458" s="2">
         <v>3</v>
       </c>
@@ -15272,7 +15272,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="459" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="459" spans="2:11">
       <c r="B459" s="2">
         <v>3</v>
       </c>
@@ -15304,7 +15304,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="460" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="460" spans="2:11">
       <c r="B460" s="2">
         <v>3</v>
       </c>
@@ -15336,7 +15336,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="461" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="461" spans="2:11">
       <c r="B461" s="2">
         <v>3</v>
       </c>
@@ -15368,7 +15368,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="462" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="462" spans="2:11">
       <c r="B462" s="2">
         <v>3</v>
       </c>
@@ -15400,7 +15400,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="463" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="463" spans="2:11">
       <c r="B463" s="2">
         <v>3</v>
       </c>
@@ -15432,7 +15432,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="464" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="464" spans="2:11">
       <c r="B464" s="2">
         <v>3</v>
       </c>
@@ -15464,7 +15464,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="465" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="465" spans="2:11">
       <c r="B465" s="2">
         <v>3</v>
       </c>
@@ -15496,7 +15496,7 @@
         <v>13.233173681010607</v>
       </c>
     </row>
-    <row r="466" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="466" spans="2:11">
       <c r="B466" s="2">
         <v>3</v>
       </c>
@@ -15528,7 +15528,7 @@
         <v>13.639999999999999</v>
       </c>
     </row>
-    <row r="467" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="467" spans="2:11">
       <c r="B467" s="2">
         <v>3</v>
       </c>
@@ -15560,7 +15560,7 @@
         <v>12.561352935232899</v>
       </c>
     </row>
-    <row r="468" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="468" spans="2:11">
       <c r="B468" s="2">
         <v>3</v>
       </c>
@@ -15592,7 +15592,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="469" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="469" spans="2:11">
       <c r="B469" s="2">
         <v>3</v>
       </c>
@@ -15624,7 +15624,7 @@
         <v>14.1</v>
       </c>
     </row>
-    <row r="470" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="470" spans="2:11">
       <c r="B470" s="2">
         <v>3</v>
       </c>
@@ -15656,7 +15656,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="471" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="471" spans="2:11">
       <c r="B471" s="2">
         <v>3</v>
       </c>
@@ -15688,7 +15688,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="472" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="472" spans="2:11">
       <c r="B472" s="2">
         <v>3</v>
       </c>
@@ -15720,7 +15720,7 @@
         <v>14.020000000000001</v>
       </c>
     </row>
-    <row r="473" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="473" spans="2:11">
       <c r="B473" s="2">
         <v>3</v>
       </c>
@@ -15752,7 +15752,7 @@
         <v>13.65</v>
       </c>
     </row>
-    <row r="474" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="474" spans="2:11">
       <c r="B474" s="2">
         <v>3</v>
       </c>
@@ -15784,7 +15784,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="475" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="475" spans="2:11">
       <c r="B475" s="2">
         <v>3</v>
       </c>
@@ -15816,7 +15816,7 @@
         <v>13.939584438549954</v>
       </c>
     </row>
-    <row r="476" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="476" spans="2:11">
       <c r="B476" s="2">
         <v>3</v>
       </c>
@@ -15848,7 +15848,7 @@
         <v>14.46470168513739</v>
       </c>
     </row>
-    <row r="477" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="477" spans="2:11">
       <c r="B477" s="2">
         <v>3</v>
       </c>
@@ -15880,7 +15880,7 @@
         <v>14.53</v>
       </c>
     </row>
-    <row r="478" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="478" spans="2:11">
       <c r="B478" s="2">
         <v>3</v>
       </c>
@@ -15912,7 +15912,7 @@
         <v>13.799999999999997</v>
       </c>
     </row>
-    <row r="479" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="479" spans="2:11">
       <c r="B479" s="2">
         <v>4</v>
       </c>
@@ -15944,7 +15944,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="480" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="480" spans="2:11">
       <c r="B480" s="2">
         <v>4</v>
       </c>
@@ -15976,7 +15976,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="481" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="481" spans="2:11">
       <c r="B481" s="2">
         <v>4</v>
       </c>
@@ -16008,7 +16008,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="482" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="482" spans="2:11">
       <c r="B482" s="2">
         <v>4</v>
       </c>
@@ -16040,7 +16040,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="483" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="483" spans="2:11">
       <c r="B483" s="2">
         <v>4</v>
       </c>
@@ -16072,7 +16072,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="484" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="484" spans="2:11">
       <c r="B484" s="2">
         <v>4</v>
       </c>
@@ -16104,7 +16104,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="485" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="485" spans="2:11">
       <c r="B485" s="2">
         <v>4</v>
       </c>
@@ -16136,7 +16136,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="486" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="486" spans="2:11">
       <c r="B486" s="2">
         <v>4</v>
       </c>
@@ -16168,7 +16168,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="487" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="487" spans="2:11">
       <c r="B487" s="2">
         <v>4</v>
       </c>
@@ -16200,7 +16200,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="488" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="488" spans="2:11">
       <c r="B488" s="2">
         <v>4</v>
       </c>
@@ -16232,7 +16232,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="489" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="489" spans="2:11">
       <c r="B489" s="2">
         <v>4</v>
       </c>
@@ -16264,7 +16264,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="490" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="490" spans="2:11">
       <c r="B490" s="2">
         <v>4</v>
       </c>
@@ -16296,7 +16296,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="491" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="491" spans="2:11">
       <c r="B491" s="2">
         <v>4</v>
       </c>
@@ -16328,7 +16328,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="492" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="492" spans="2:11">
       <c r="B492" s="2">
         <v>4</v>
       </c>
@@ -16360,7 +16360,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="493" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="493" spans="2:11">
       <c r="B493" s="2">
         <v>4</v>
       </c>
@@ -16392,7 +16392,7 @@
         <v>13.59</v>
       </c>
     </row>
-    <row r="494" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="494" spans="2:11">
       <c r="B494" s="2">
         <v>4</v>
       </c>
@@ -16424,7 +16424,7 @@
         <v>13.93</v>
       </c>
     </row>
-    <row r="495" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="495" spans="2:11">
       <c r="B495" s="2">
         <v>4</v>
       </c>
@@ -16456,7 +16456,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="496" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="496" spans="2:11">
       <c r="B496" s="2">
         <v>4</v>
       </c>
@@ -16488,7 +16488,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="497" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="497" spans="2:11">
       <c r="B497" s="2">
         <v>4</v>
       </c>
@@ -16520,7 +16520,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="498" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="498" spans="2:11">
       <c r="B498" s="2">
         <v>4</v>
       </c>
@@ -16552,7 +16552,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="499" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="499" spans="2:11">
       <c r="B499" s="2">
         <v>4</v>
       </c>
@@ -16584,7 +16584,7 @@
         <v>14.12</v>
       </c>
     </row>
-    <row r="500" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="500" spans="2:11">
       <c r="B500" s="2">
         <v>4</v>
       </c>
@@ -16616,7 +16616,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="501" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="501" spans="2:11">
       <c r="B501" s="2">
         <v>4</v>
       </c>
@@ -16648,7 +16648,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="502" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="502" spans="2:11">
       <c r="B502" s="2">
         <v>4</v>
       </c>
@@ -16680,7 +16680,7 @@
         <v>13.998170075349838</v>
       </c>
     </row>
-    <row r="503" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="503" spans="2:11">
       <c r="B503" s="2">
         <v>4</v>
       </c>
@@ -16712,7 +16712,7 @@
         <v>14.428119469026548</v>
       </c>
     </row>
-    <row r="504" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="504" spans="2:11">
       <c r="B504" s="2">
         <v>4</v>
       </c>
@@ -16744,7 +16744,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="505" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="505" spans="2:11">
       <c r="B505" s="2">
         <v>4</v>
       </c>
@@ -16776,7 +16776,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="506" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="506" spans="2:11">
       <c r="B506" s="2">
         <v>4</v>
       </c>

</xml_diff>